<commit_message>
2511220213 - No "O" and Row Colors
</commit_message>
<xml_diff>
--- a/backend/docs/How Oportunities will be showed on Table.xlsx
+++ b/backend/docs/How Oportunities will be showed on Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Other computers\My Computer\Documents\GitHub\Put-Oportunity-Finder\backend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A7F81D1-8979-4936-98CD-84BBC25ABF6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8623F5FB-1563-47F4-9AF5-137DE161B85C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="4430" windowWidth="25740" windowHeight="9930" xr2:uid="{AD6F44AE-3219-46C7-9A01-3ECF2A281AE2}"/>
   </bookViews>
@@ -131,13 +131,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -171,24 +171,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -531,7 +531,7 @@
   <dimension ref="B8:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:N16"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -546,36 +546,36 @@
     <col min="14" max="14" width="45.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="2:14" s="6" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="B8" s="5" t="s">
+    <row r="8" spans="2:14" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="H8" s="8" t="s">
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="H8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L8" s="9" t="s">
+      <c r="L8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="N8" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:14" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="D9" s="10" t="s">
+    <row r="9" spans="2:14" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="D9" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -612,7 +612,7 @@
         <v>4</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="H13" s="3"/>
+      <c r="H13" s="10"/>
       <c r="L13" t="s">
         <v>13</v>
       </c>
@@ -628,7 +628,7 @@
       <c r="F14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H14" s="3"/>
+      <c r="H14" s="10"/>
       <c r="L14" t="s">
         <v>13</v>
       </c>
@@ -646,7 +646,7 @@
       <c r="F15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="4"/>
+      <c r="H15" s="9"/>
       <c r="J15" s="1" t="s">
         <v>6</v>
       </c>
@@ -667,7 +667,7 @@
       <c r="F16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="4"/>
+      <c r="H16" s="9"/>
       <c r="J16" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
2511220237 - New Row Colors
</commit_message>
<xml_diff>
--- a/backend/docs/How Oportunities will be showed on Table.xlsx
+++ b/backend/docs/How Oportunities will be showed on Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Other computers\My Computer\Documents\GitHub\Put-Oportunity-Finder\backend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8623F5FB-1563-47F4-9AF5-137DE161B85C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DF1770-4DA8-4EFC-BB14-554EF6F9D809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="4430" windowWidth="25740" windowHeight="9930" xr2:uid="{AD6F44AE-3219-46C7-9A01-3ECF2A281AE2}"/>
   </bookViews>
@@ -125,19 +125,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -168,9 +168,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -180,6 +177,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -531,7 +531,7 @@
   <dimension ref="B8:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -546,8 +546,8 @@
     <col min="14" max="14" width="45.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="2:14" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
+    <row r="8" spans="2:14" s="3" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="8" t="s">
@@ -555,27 +555,27 @@
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="L8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="N8" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:14" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="D9" s="7" t="s">
+    <row r="9" spans="2:14" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="D9" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>2</v>
       </c>
     </row>
@@ -596,7 +596,7 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="H12" s="2"/>
+      <c r="H12" s="10"/>
       <c r="L12" t="s">
         <v>13</v>
       </c>
@@ -612,7 +612,7 @@
         <v>4</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="H13" s="10"/>
+      <c r="H13" s="9"/>
       <c r="L13" t="s">
         <v>13</v>
       </c>
@@ -628,7 +628,7 @@
       <c r="F14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H14" s="10"/>
+      <c r="H14" s="9"/>
       <c r="L14" t="s">
         <v>13</v>
       </c>
@@ -646,7 +646,7 @@
       <c r="F15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="9"/>
+      <c r="H15" s="7"/>
       <c r="J15" s="1" t="s">
         <v>6</v>
       </c>
@@ -667,7 +667,7 @@
       <c r="F16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="9"/>
+      <c r="H16" s="7"/>
       <c r="J16" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>